<commit_message>
fixed the freezr and timer
</commit_message>
<xml_diff>
--- a/db_tables/spaceshipResults.xlsx
+++ b/db_tables/spaceshipResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,12 @@
     <t>cb</t>
   </si>
   <si>
+    <t>Moshe</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>user1</t>
   </si>
   <si>
@@ -110,7 +116,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>14</t>
+    <t>20</t>
   </si>
   <si>
     <t>ad</t>
@@ -122,7 +128,7 @@
     <t>Erez</t>
   </si>
   <si>
-    <t>11</t>
+    <t>110</t>
   </si>
   <si>
     <t>test</t>
@@ -141,6 +147,9 @@
   </si>
   <si>
     <t>bjnm</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
   <si>
     <t>sdfs</t>
@@ -233,7 +242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:CV45"/>
+  <dimension ref="A1:CV47"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2478,7 +2487,7 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2581,10 +2590,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -2687,10 +2696,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -2796,7 +2805,7 @@
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -2899,10 +2908,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -3005,7 +3014,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -3111,7 +3120,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -3217,7 +3226,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -3323,7 +3332,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -3429,10 +3438,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -3535,10 +3544,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -3641,10 +3650,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -3747,10 +3756,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
@@ -3853,7 +3862,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -3959,10 +3968,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -4068,7 +4077,7 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C38"/>
       <c r="D38"/>
@@ -4174,7 +4183,7 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
@@ -4277,10 +4286,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -4383,7 +4392,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
@@ -4489,10 +4498,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C42"/>
       <c r="D42"/>
@@ -4595,7 +4604,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
@@ -4701,10 +4710,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C44"/>
       <c r="D44"/>
@@ -4911,6 +4920,218 @@
       <c r="CU45"/>
       <c r="CV45"/>
     </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+      <c r="Y46"/>
+      <c r="Z46"/>
+      <c r="AA46"/>
+      <c r="AB46"/>
+      <c r="AC46"/>
+      <c r="AD46"/>
+      <c r="AE46"/>
+      <c r="AF46"/>
+      <c r="AG46"/>
+      <c r="AH46"/>
+      <c r="AI46"/>
+      <c r="AJ46"/>
+      <c r="AK46"/>
+      <c r="AL46"/>
+      <c r="AM46"/>
+      <c r="AN46"/>
+      <c r="AO46"/>
+      <c r="AP46"/>
+      <c r="AQ46"/>
+      <c r="AR46"/>
+      <c r="AS46"/>
+      <c r="AT46"/>
+      <c r="AU46"/>
+      <c r="AV46"/>
+      <c r="AW46"/>
+      <c r="AX46"/>
+      <c r="AY46"/>
+      <c r="AZ46"/>
+      <c r="BA46"/>
+      <c r="BB46"/>
+      <c r="BC46"/>
+      <c r="BD46"/>
+      <c r="BE46"/>
+      <c r="BF46"/>
+      <c r="BG46"/>
+      <c r="BH46"/>
+      <c r="BI46"/>
+      <c r="BJ46"/>
+      <c r="BK46"/>
+      <c r="BL46"/>
+      <c r="BM46"/>
+      <c r="BN46"/>
+      <c r="BO46"/>
+      <c r="BP46"/>
+      <c r="BQ46"/>
+      <c r="BR46"/>
+      <c r="BS46"/>
+      <c r="BT46"/>
+      <c r="BU46"/>
+      <c r="BV46"/>
+      <c r="BW46"/>
+      <c r="BX46"/>
+      <c r="BY46"/>
+      <c r="BZ46"/>
+      <c r="CA46"/>
+      <c r="CB46"/>
+      <c r="CC46"/>
+      <c r="CD46"/>
+      <c r="CE46"/>
+      <c r="CF46"/>
+      <c r="CG46"/>
+      <c r="CH46"/>
+      <c r="CI46"/>
+      <c r="CJ46"/>
+      <c r="CK46"/>
+      <c r="CL46"/>
+      <c r="CM46"/>
+      <c r="CN46"/>
+      <c r="CO46"/>
+      <c r="CP46"/>
+      <c r="CQ46"/>
+      <c r="CR46"/>
+      <c r="CS46"/>
+      <c r="CT46"/>
+      <c r="CU46"/>
+      <c r="CV46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+      <c r="Z47"/>
+      <c r="AA47"/>
+      <c r="AB47"/>
+      <c r="AC47"/>
+      <c r="AD47"/>
+      <c r="AE47"/>
+      <c r="AF47"/>
+      <c r="AG47"/>
+      <c r="AH47"/>
+      <c r="AI47"/>
+      <c r="AJ47"/>
+      <c r="AK47"/>
+      <c r="AL47"/>
+      <c r="AM47"/>
+      <c r="AN47"/>
+      <c r="AO47"/>
+      <c r="AP47"/>
+      <c r="AQ47"/>
+      <c r="AR47"/>
+      <c r="AS47"/>
+      <c r="AT47"/>
+      <c r="AU47"/>
+      <c r="AV47"/>
+      <c r="AW47"/>
+      <c r="AX47"/>
+      <c r="AY47"/>
+      <c r="AZ47"/>
+      <c r="BA47"/>
+      <c r="BB47"/>
+      <c r="BC47"/>
+      <c r="BD47"/>
+      <c r="BE47"/>
+      <c r="BF47"/>
+      <c r="BG47"/>
+      <c r="BH47"/>
+      <c r="BI47"/>
+      <c r="BJ47"/>
+      <c r="BK47"/>
+      <c r="BL47"/>
+      <c r="BM47"/>
+      <c r="BN47"/>
+      <c r="BO47"/>
+      <c r="BP47"/>
+      <c r="BQ47"/>
+      <c r="BR47"/>
+      <c r="BS47"/>
+      <c r="BT47"/>
+      <c r="BU47"/>
+      <c r="BV47"/>
+      <c r="BW47"/>
+      <c r="BX47"/>
+      <c r="BY47"/>
+      <c r="BZ47"/>
+      <c r="CA47"/>
+      <c r="CB47"/>
+      <c r="CC47"/>
+      <c r="CD47"/>
+      <c r="CE47"/>
+      <c r="CF47"/>
+      <c r="CG47"/>
+      <c r="CH47"/>
+      <c r="CI47"/>
+      <c r="CJ47"/>
+      <c r="CK47"/>
+      <c r="CL47"/>
+      <c r="CM47"/>
+      <c r="CN47"/>
+      <c r="CO47"/>
+      <c r="CP47"/>
+      <c r="CQ47"/>
+      <c r="CR47"/>
+      <c r="CS47"/>
+      <c r="CT47"/>
+      <c r="CU47"/>
+      <c r="CV47"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
stable version rand freezer
</commit_message>
<xml_diff>
--- a/db_tables/spaceshipResults.xlsx
+++ b/db_tables/spaceshipResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -188,10 +188,16 @@
     <t>j</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>sdfs</t>
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
   <si>
     <t>m</t>
@@ -269,7 +275,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:CV54"/>
+  <dimension ref="A1:CV55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2410,6 +2416,104 @@
       <c r="B22" t="s">
         <v>29</v>
       </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
+      <c r="BG22"/>
+      <c r="BH22"/>
+      <c r="BI22"/>
+      <c r="BJ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
+      <c r="BM22"/>
+      <c r="BN22"/>
+      <c r="BO22"/>
+      <c r="BP22"/>
+      <c r="BQ22"/>
+      <c r="BR22"/>
+      <c r="BS22"/>
+      <c r="BT22"/>
+      <c r="BU22"/>
+      <c r="BV22"/>
+      <c r="BW22"/>
+      <c r="BX22"/>
+      <c r="BY22"/>
+      <c r="BZ22"/>
+      <c r="CA22"/>
+      <c r="CB22"/>
+      <c r="CC22"/>
+      <c r="CD22"/>
+      <c r="CE22"/>
+      <c r="CF22"/>
+      <c r="CG22"/>
+      <c r="CH22"/>
+      <c r="CI22"/>
+      <c r="CJ22"/>
+      <c r="CK22"/>
+      <c r="CL22"/>
+      <c r="CM22"/>
+      <c r="CN22"/>
+      <c r="CO22"/>
+      <c r="CP22"/>
+      <c r="CQ22"/>
+      <c r="CR22"/>
+      <c r="CS22"/>
+      <c r="CT22"/>
+      <c r="CU22"/>
+      <c r="CV22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -4430,7 +4534,7 @@
         <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C42"/>
       <c r="D42"/>
@@ -4533,7 +4637,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -4639,7 +4743,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -4745,10 +4849,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C45"/>
       <c r="D45"/>
@@ -4851,10 +4955,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C46"/>
       <c r="D46"/>
@@ -4957,10 +5061,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C47"/>
       <c r="D47"/>
@@ -5063,10 +5167,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C48"/>
       <c r="D48"/>
@@ -5169,7 +5273,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -5275,7 +5379,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -5381,10 +5485,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -5487,10 +5591,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C52"/>
       <c r="D52"/>
@@ -5593,10 +5697,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="C53"/>
       <c r="D53"/>
@@ -5702,7 +5806,7 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C54"/>
       <c r="D54"/>
@@ -5803,6 +5907,112 @@
       <c r="CU54"/>
       <c r="CV54"/>
     </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+      <c r="Y55"/>
+      <c r="Z55"/>
+      <c r="AA55"/>
+      <c r="AB55"/>
+      <c r="AC55"/>
+      <c r="AD55"/>
+      <c r="AE55"/>
+      <c r="AF55"/>
+      <c r="AG55"/>
+      <c r="AH55"/>
+      <c r="AI55"/>
+      <c r="AJ55"/>
+      <c r="AK55"/>
+      <c r="AL55"/>
+      <c r="AM55"/>
+      <c r="AN55"/>
+      <c r="AO55"/>
+      <c r="AP55"/>
+      <c r="AQ55"/>
+      <c r="AR55"/>
+      <c r="AS55"/>
+      <c r="AT55"/>
+      <c r="AU55"/>
+      <c r="AV55"/>
+      <c r="AW55"/>
+      <c r="AX55"/>
+      <c r="AY55"/>
+      <c r="AZ55"/>
+      <c r="BA55"/>
+      <c r="BB55"/>
+      <c r="BC55"/>
+      <c r="BD55"/>
+      <c r="BE55"/>
+      <c r="BF55"/>
+      <c r="BG55"/>
+      <c r="BH55"/>
+      <c r="BI55"/>
+      <c r="BJ55"/>
+      <c r="BK55"/>
+      <c r="BL55"/>
+      <c r="BM55"/>
+      <c r="BN55"/>
+      <c r="BO55"/>
+      <c r="BP55"/>
+      <c r="BQ55"/>
+      <c r="BR55"/>
+      <c r="BS55"/>
+      <c r="BT55"/>
+      <c r="BU55"/>
+      <c r="BV55"/>
+      <c r="BW55"/>
+      <c r="BX55"/>
+      <c r="BY55"/>
+      <c r="BZ55"/>
+      <c r="CA55"/>
+      <c r="CB55"/>
+      <c r="CC55"/>
+      <c r="CD55"/>
+      <c r="CE55"/>
+      <c r="CF55"/>
+      <c r="CG55"/>
+      <c r="CH55"/>
+      <c r="CI55"/>
+      <c r="CJ55"/>
+      <c r="CK55"/>
+      <c r="CL55"/>
+      <c r="CM55"/>
+      <c r="CN55"/>
+      <c r="CO55"/>
+      <c r="CP55"/>
+      <c r="CQ55"/>
+      <c r="CR55"/>
+      <c r="CS55"/>
+      <c r="CT55"/>
+      <c r="CU55"/>
+      <c r="CV55"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
stable version with dagonal movment
</commit_message>
<xml_diff>
--- a/db_tables/spaceshipResults.xlsx
+++ b/db_tables/spaceshipResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -26,6 +26,12 @@
     <t>1</t>
   </si>
   <si>
+    <t>EREZ</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
     <t>ohad</t>
   </si>
   <si>
@@ -168,6 +174,12 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>f</t>
@@ -275,7 +287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:CV55"/>
+  <dimension ref="A1:CV58"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -402,104 +414,6 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-      <c r="AF3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-      <c r="AS3"/>
-      <c r="AT3"/>
-      <c r="AU3"/>
-      <c r="AV3"/>
-      <c r="AW3"/>
-      <c r="AX3"/>
-      <c r="AY3"/>
-      <c r="AZ3"/>
-      <c r="BA3"/>
-      <c r="BB3"/>
-      <c r="BC3"/>
-      <c r="BD3"/>
-      <c r="BE3"/>
-      <c r="BF3"/>
-      <c r="BG3"/>
-      <c r="BH3"/>
-      <c r="BI3"/>
-      <c r="BJ3"/>
-      <c r="BK3"/>
-      <c r="BL3"/>
-      <c r="BM3"/>
-      <c r="BN3"/>
-      <c r="BO3"/>
-      <c r="BP3"/>
-      <c r="BQ3"/>
-      <c r="BR3"/>
-      <c r="BS3"/>
-      <c r="BT3"/>
-      <c r="BU3"/>
-      <c r="BV3"/>
-      <c r="BW3"/>
-      <c r="BX3"/>
-      <c r="BY3"/>
-      <c r="BZ3"/>
-      <c r="CA3"/>
-      <c r="CB3"/>
-      <c r="CC3"/>
-      <c r="CD3"/>
-      <c r="CE3"/>
-      <c r="CF3"/>
-      <c r="CG3"/>
-      <c r="CH3"/>
-      <c r="CI3"/>
-      <c r="CJ3"/>
-      <c r="CK3"/>
-      <c r="CL3"/>
-      <c r="CM3"/>
-      <c r="CN3"/>
-      <c r="CO3"/>
-      <c r="CP3"/>
-      <c r="CQ3"/>
-      <c r="CR3"/>
-      <c r="CS3"/>
-      <c r="CT3"/>
-      <c r="CU3"/>
-      <c r="CV3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -612,7 +526,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -715,10 +629,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -824,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -927,10 +841,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -1033,10 +947,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -1142,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -1245,10 +1159,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -1351,10 +1265,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -1457,10 +1371,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -1566,7 +1480,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -1669,10 +1583,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -1775,10 +1689,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -1881,10 +1795,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -1987,10 +1901,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
@@ -2093,10 +2007,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -2199,10 +2113,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2305,10 +2219,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -2411,10 +2325,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
@@ -2520,7 +2434,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2623,10 +2537,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -2729,10 +2643,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -2838,7 +2752,7 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -2941,10 +2855,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -3047,10 +2961,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -3156,7 +3070,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -3259,10 +3173,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -3368,7 +3282,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -3471,10 +3385,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -3580,7 +3494,7 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -3683,10 +3597,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -3898,7 +3812,7 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C36"/>
       <c r="D36"/>
@@ -4001,10 +3915,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -4216,7 +4130,7 @@
         <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
@@ -4322,7 +4236,7 @@
         <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -4428,7 +4342,7 @@
         <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C41"/>
       <c r="D41"/>
@@ -4531,10 +4445,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C42"/>
       <c r="D42"/>
@@ -4640,7 +4554,7 @@
         <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C43"/>
       <c r="D43"/>
@@ -4746,7 +4660,7 @@
         <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C44"/>
       <c r="D44"/>
@@ -4852,7 +4766,7 @@
         <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C45"/>
       <c r="D45"/>
@@ -4955,10 +4869,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C46"/>
       <c r="D46"/>
@@ -5061,10 +4975,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C47"/>
       <c r="D47"/>
@@ -5167,10 +5081,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C48"/>
       <c r="D48"/>
@@ -5273,10 +5187,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C49"/>
       <c r="D49"/>
@@ -5379,10 +5293,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C50"/>
       <c r="D50"/>
@@ -5485,10 +5399,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -5591,10 +5505,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C52"/>
       <c r="D52"/>
@@ -5697,10 +5611,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C53"/>
       <c r="D53"/>
@@ -5803,10 +5717,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C54"/>
       <c r="D54"/>
@@ -5912,7 +5826,7 @@
         <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C55"/>
       <c r="D55"/>
@@ -6013,6 +5927,324 @@
       <c r="CU55"/>
       <c r="CV55"/>
     </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+      <c r="U56"/>
+      <c r="V56"/>
+      <c r="W56"/>
+      <c r="X56"/>
+      <c r="Y56"/>
+      <c r="Z56"/>
+      <c r="AA56"/>
+      <c r="AB56"/>
+      <c r="AC56"/>
+      <c r="AD56"/>
+      <c r="AE56"/>
+      <c r="AF56"/>
+      <c r="AG56"/>
+      <c r="AH56"/>
+      <c r="AI56"/>
+      <c r="AJ56"/>
+      <c r="AK56"/>
+      <c r="AL56"/>
+      <c r="AM56"/>
+      <c r="AN56"/>
+      <c r="AO56"/>
+      <c r="AP56"/>
+      <c r="AQ56"/>
+      <c r="AR56"/>
+      <c r="AS56"/>
+      <c r="AT56"/>
+      <c r="AU56"/>
+      <c r="AV56"/>
+      <c r="AW56"/>
+      <c r="AX56"/>
+      <c r="AY56"/>
+      <c r="AZ56"/>
+      <c r="BA56"/>
+      <c r="BB56"/>
+      <c r="BC56"/>
+      <c r="BD56"/>
+      <c r="BE56"/>
+      <c r="BF56"/>
+      <c r="BG56"/>
+      <c r="BH56"/>
+      <c r="BI56"/>
+      <c r="BJ56"/>
+      <c r="BK56"/>
+      <c r="BL56"/>
+      <c r="BM56"/>
+      <c r="BN56"/>
+      <c r="BO56"/>
+      <c r="BP56"/>
+      <c r="BQ56"/>
+      <c r="BR56"/>
+      <c r="BS56"/>
+      <c r="BT56"/>
+      <c r="BU56"/>
+      <c r="BV56"/>
+      <c r="BW56"/>
+      <c r="BX56"/>
+      <c r="BY56"/>
+      <c r="BZ56"/>
+      <c r="CA56"/>
+      <c r="CB56"/>
+      <c r="CC56"/>
+      <c r="CD56"/>
+      <c r="CE56"/>
+      <c r="CF56"/>
+      <c r="CG56"/>
+      <c r="CH56"/>
+      <c r="CI56"/>
+      <c r="CJ56"/>
+      <c r="CK56"/>
+      <c r="CL56"/>
+      <c r="CM56"/>
+      <c r="CN56"/>
+      <c r="CO56"/>
+      <c r="CP56"/>
+      <c r="CQ56"/>
+      <c r="CR56"/>
+      <c r="CS56"/>
+      <c r="CT56"/>
+      <c r="CU56"/>
+      <c r="CV56"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+      <c r="U57"/>
+      <c r="V57"/>
+      <c r="W57"/>
+      <c r="X57"/>
+      <c r="Y57"/>
+      <c r="Z57"/>
+      <c r="AA57"/>
+      <c r="AB57"/>
+      <c r="AC57"/>
+      <c r="AD57"/>
+      <c r="AE57"/>
+      <c r="AF57"/>
+      <c r="AG57"/>
+      <c r="AH57"/>
+      <c r="AI57"/>
+      <c r="AJ57"/>
+      <c r="AK57"/>
+      <c r="AL57"/>
+      <c r="AM57"/>
+      <c r="AN57"/>
+      <c r="AO57"/>
+      <c r="AP57"/>
+      <c r="AQ57"/>
+      <c r="AR57"/>
+      <c r="AS57"/>
+      <c r="AT57"/>
+      <c r="AU57"/>
+      <c r="AV57"/>
+      <c r="AW57"/>
+      <c r="AX57"/>
+      <c r="AY57"/>
+      <c r="AZ57"/>
+      <c r="BA57"/>
+      <c r="BB57"/>
+      <c r="BC57"/>
+      <c r="BD57"/>
+      <c r="BE57"/>
+      <c r="BF57"/>
+      <c r="BG57"/>
+      <c r="BH57"/>
+      <c r="BI57"/>
+      <c r="BJ57"/>
+      <c r="BK57"/>
+      <c r="BL57"/>
+      <c r="BM57"/>
+      <c r="BN57"/>
+      <c r="BO57"/>
+      <c r="BP57"/>
+      <c r="BQ57"/>
+      <c r="BR57"/>
+      <c r="BS57"/>
+      <c r="BT57"/>
+      <c r="BU57"/>
+      <c r="BV57"/>
+      <c r="BW57"/>
+      <c r="BX57"/>
+      <c r="BY57"/>
+      <c r="BZ57"/>
+      <c r="CA57"/>
+      <c r="CB57"/>
+      <c r="CC57"/>
+      <c r="CD57"/>
+      <c r="CE57"/>
+      <c r="CF57"/>
+      <c r="CG57"/>
+      <c r="CH57"/>
+      <c r="CI57"/>
+      <c r="CJ57"/>
+      <c r="CK57"/>
+      <c r="CL57"/>
+      <c r="CM57"/>
+      <c r="CN57"/>
+      <c r="CO57"/>
+      <c r="CP57"/>
+      <c r="CQ57"/>
+      <c r="CR57"/>
+      <c r="CS57"/>
+      <c r="CT57"/>
+      <c r="CU57"/>
+      <c r="CV57"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="T58"/>
+      <c r="U58"/>
+      <c r="V58"/>
+      <c r="W58"/>
+      <c r="X58"/>
+      <c r="Y58"/>
+      <c r="Z58"/>
+      <c r="AA58"/>
+      <c r="AB58"/>
+      <c r="AC58"/>
+      <c r="AD58"/>
+      <c r="AE58"/>
+      <c r="AF58"/>
+      <c r="AG58"/>
+      <c r="AH58"/>
+      <c r="AI58"/>
+      <c r="AJ58"/>
+      <c r="AK58"/>
+      <c r="AL58"/>
+      <c r="AM58"/>
+      <c r="AN58"/>
+      <c r="AO58"/>
+      <c r="AP58"/>
+      <c r="AQ58"/>
+      <c r="AR58"/>
+      <c r="AS58"/>
+      <c r="AT58"/>
+      <c r="AU58"/>
+      <c r="AV58"/>
+      <c r="AW58"/>
+      <c r="AX58"/>
+      <c r="AY58"/>
+      <c r="AZ58"/>
+      <c r="BA58"/>
+      <c r="BB58"/>
+      <c r="BC58"/>
+      <c r="BD58"/>
+      <c r="BE58"/>
+      <c r="BF58"/>
+      <c r="BG58"/>
+      <c r="BH58"/>
+      <c r="BI58"/>
+      <c r="BJ58"/>
+      <c r="BK58"/>
+      <c r="BL58"/>
+      <c r="BM58"/>
+      <c r="BN58"/>
+      <c r="BO58"/>
+      <c r="BP58"/>
+      <c r="BQ58"/>
+      <c r="BR58"/>
+      <c r="BS58"/>
+      <c r="BT58"/>
+      <c r="BU58"/>
+      <c r="BV58"/>
+      <c r="BW58"/>
+      <c r="BX58"/>
+      <c r="BY58"/>
+      <c r="BZ58"/>
+      <c r="CA58"/>
+      <c r="CB58"/>
+      <c r="CC58"/>
+      <c r="CD58"/>
+      <c r="CE58"/>
+      <c r="CF58"/>
+      <c r="CG58"/>
+      <c r="CH58"/>
+      <c r="CI58"/>
+      <c r="CJ58"/>
+      <c r="CK58"/>
+      <c r="CL58"/>
+      <c r="CM58"/>
+      <c r="CN58"/>
+      <c r="CO58"/>
+      <c r="CP58"/>
+      <c r="CQ58"/>
+      <c r="CR58"/>
+      <c r="CS58"/>
+      <c r="CT58"/>
+      <c r="CU58"/>
+      <c r="CV58"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
last changes, new classes
</commit_message>
<xml_diff>
--- a/db_tables/spaceshipResults.xlsx
+++ b/db_tables/spaceshipResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -20,42 +20,60 @@
     <t>Result</t>
   </si>
   <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>df</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>EREZ</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>ohad</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> \c\\</t>
+  </si>
+  <si>
+    <t>grfgbfgb</t>
+  </si>
+  <si>
+    <t>erez</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>beni</t>
+  </si>
+  <si>
+    <t>erez8</t>
+  </si>
+  <si>
+    <t>erez9</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>EREZ</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>ohad</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>grfgbfgb</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>erez</t>
-  </si>
-  <si>
-    <t>erez8</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>erez9</t>
-  </si>
-  <si>
     <t>Ariel</t>
   </si>
   <si>
@@ -65,6 +83,18 @@
     <t>6</t>
   </si>
   <si>
+    <t xml:space="preserve"> lj</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>ad</t>
   </si>
   <si>
@@ -77,9 +107,6 @@
     <t>ljk</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>vc</t>
   </si>
   <si>
@@ -92,6 +119,24 @@
     <t>dfs</t>
   </si>
   <si>
+    <t>vg</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>Avi</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>dsf</t>
   </si>
   <si>
@@ -104,6 +149,12 @@
     <t>fg</t>
   </si>
   <si>
+    <t>,m</t>
+  </si>
+  <si>
+    <t>csda</t>
+  </si>
+  <si>
     <t>J</t>
   </si>
   <si>
@@ -122,6 +173,9 @@
     <t>5</t>
   </si>
   <si>
+    <t>fv</t>
+  </si>
+  <si>
     <t>sd</t>
   </si>
   <si>
@@ -140,9 +194,6 @@
     <t>Sorin</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>cb</t>
   </si>
   <si>
@@ -155,16 +206,22 @@
     <t>kj</t>
   </si>
   <si>
+    <t>ששש</t>
+  </si>
+  <si>
     <t>user1</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
+    <t>bhg</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
-    <t>20</t>
+    <t>b</t>
   </si>
   <si>
     <t>c</t>
@@ -194,6 +251,9 @@
     <t>g</t>
   </si>
   <si>
+    <t>h</t>
+  </si>
+  <si>
     <t>i</t>
   </si>
   <si>
@@ -218,22 +278,40 @@
     <t>xf</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>neta G</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
     <t>s</t>
   </si>
   <si>
+    <t>cv</t>
+  </si>
+  <si>
     <t>t</t>
   </si>
   <si>
+    <t>דגכדג</t>
+  </si>
+  <si>
     <t>v</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
+    <t>sdasedfeasfsd</t>
+  </si>
+  <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>xs</t>
   </si>
   <si>
     <t>user100</t>
@@ -287,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:CV58"/>
+  <dimension ref="A1:CV83"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -414,6 +492,104 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
+      <c r="CJ3"/>
+      <c r="CK3"/>
+      <c r="CL3"/>
+      <c r="CM3"/>
+      <c r="CN3"/>
+      <c r="CO3"/>
+      <c r="CP3"/>
+      <c r="CQ3"/>
+      <c r="CR3"/>
+      <c r="CS3"/>
+      <c r="CT3"/>
+      <c r="CU3"/>
+      <c r="CV3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -632,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -738,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -841,10 +1017,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -950,7 +1126,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -1053,10 +1229,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -1162,7 +1338,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -1268,7 +1444,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -1371,10 +1547,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -1477,10 +1653,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -1583,10 +1759,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -1689,10 +1865,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -1795,10 +1971,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -1901,10 +2077,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
@@ -2007,10 +2183,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -2113,10 +2289,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2219,10 +2395,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -2325,10 +2501,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
@@ -2431,10 +2607,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2537,10 +2713,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -2643,10 +2819,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -2749,10 +2925,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -2858,7 +3034,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -2964,7 +3140,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -3070,7 +3246,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -3173,10 +3349,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>40</v>
-      </c>
-      <c r="B30" t="s">
-        <v>12</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -3282,7 +3458,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -3385,10 +3561,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -3491,10 +3667,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -3597,10 +3773,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -3703,10 +3879,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
@@ -3809,10 +3985,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C36"/>
       <c r="D36"/>
@@ -3915,10 +4091,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -4021,10 +4197,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C38"/>
       <c r="D38"/>
@@ -4127,10 +4303,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
@@ -4233,10 +4409,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -4339,10 +4515,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C41"/>
       <c r="D41"/>
@@ -4445,10 +4621,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C42"/>
       <c r="D42"/>
@@ -4551,10 +4727,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C43"/>
       <c r="D43"/>
@@ -4657,10 +4833,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C44"/>
       <c r="D44"/>
@@ -4763,10 +4939,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C45"/>
       <c r="D45"/>
@@ -4869,10 +5045,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C46"/>
       <c r="D46"/>
@@ -4975,10 +5151,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C47"/>
       <c r="D47"/>
@@ -5081,10 +5257,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C48"/>
       <c r="D48"/>
@@ -5187,10 +5363,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C49"/>
       <c r="D49"/>
@@ -5293,10 +5469,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C50"/>
       <c r="D50"/>
@@ -5399,10 +5575,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -5505,10 +5681,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C52"/>
       <c r="D52"/>
@@ -5611,10 +5787,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C53"/>
       <c r="D53"/>
@@ -5717,10 +5893,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C54"/>
       <c r="D54"/>
@@ -5823,10 +5999,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C55"/>
       <c r="D55"/>
@@ -5929,10 +6105,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="C56"/>
       <c r="D56"/>
@@ -6035,10 +6211,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C57"/>
       <c r="D57"/>
@@ -6141,10 +6317,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C58"/>
       <c r="D58"/>
@@ -6245,6 +6421,2656 @@
       <c r="CU58"/>
       <c r="CV58"/>
     </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59"/>
+      <c r="Y59"/>
+      <c r="Z59"/>
+      <c r="AA59"/>
+      <c r="AB59"/>
+      <c r="AC59"/>
+      <c r="AD59"/>
+      <c r="AE59"/>
+      <c r="AF59"/>
+      <c r="AG59"/>
+      <c r="AH59"/>
+      <c r="AI59"/>
+      <c r="AJ59"/>
+      <c r="AK59"/>
+      <c r="AL59"/>
+      <c r="AM59"/>
+      <c r="AN59"/>
+      <c r="AO59"/>
+      <c r="AP59"/>
+      <c r="AQ59"/>
+      <c r="AR59"/>
+      <c r="AS59"/>
+      <c r="AT59"/>
+      <c r="AU59"/>
+      <c r="AV59"/>
+      <c r="AW59"/>
+      <c r="AX59"/>
+      <c r="AY59"/>
+      <c r="AZ59"/>
+      <c r="BA59"/>
+      <c r="BB59"/>
+      <c r="BC59"/>
+      <c r="BD59"/>
+      <c r="BE59"/>
+      <c r="BF59"/>
+      <c r="BG59"/>
+      <c r="BH59"/>
+      <c r="BI59"/>
+      <c r="BJ59"/>
+      <c r="BK59"/>
+      <c r="BL59"/>
+      <c r="BM59"/>
+      <c r="BN59"/>
+      <c r="BO59"/>
+      <c r="BP59"/>
+      <c r="BQ59"/>
+      <c r="BR59"/>
+      <c r="BS59"/>
+      <c r="BT59"/>
+      <c r="BU59"/>
+      <c r="BV59"/>
+      <c r="BW59"/>
+      <c r="BX59"/>
+      <c r="BY59"/>
+      <c r="BZ59"/>
+      <c r="CA59"/>
+      <c r="CB59"/>
+      <c r="CC59"/>
+      <c r="CD59"/>
+      <c r="CE59"/>
+      <c r="CF59"/>
+      <c r="CG59"/>
+      <c r="CH59"/>
+      <c r="CI59"/>
+      <c r="CJ59"/>
+      <c r="CK59"/>
+      <c r="CL59"/>
+      <c r="CM59"/>
+      <c r="CN59"/>
+      <c r="CO59"/>
+      <c r="CP59"/>
+      <c r="CQ59"/>
+      <c r="CR59"/>
+      <c r="CS59"/>
+      <c r="CT59"/>
+      <c r="CU59"/>
+      <c r="CV59"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+      <c r="Y60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
+      <c r="AC60"/>
+      <c r="AD60"/>
+      <c r="AE60"/>
+      <c r="AF60"/>
+      <c r="AG60"/>
+      <c r="AH60"/>
+      <c r="AI60"/>
+      <c r="AJ60"/>
+      <c r="AK60"/>
+      <c r="AL60"/>
+      <c r="AM60"/>
+      <c r="AN60"/>
+      <c r="AO60"/>
+      <c r="AP60"/>
+      <c r="AQ60"/>
+      <c r="AR60"/>
+      <c r="AS60"/>
+      <c r="AT60"/>
+      <c r="AU60"/>
+      <c r="AV60"/>
+      <c r="AW60"/>
+      <c r="AX60"/>
+      <c r="AY60"/>
+      <c r="AZ60"/>
+      <c r="BA60"/>
+      <c r="BB60"/>
+      <c r="BC60"/>
+      <c r="BD60"/>
+      <c r="BE60"/>
+      <c r="BF60"/>
+      <c r="BG60"/>
+      <c r="BH60"/>
+      <c r="BI60"/>
+      <c r="BJ60"/>
+      <c r="BK60"/>
+      <c r="BL60"/>
+      <c r="BM60"/>
+      <c r="BN60"/>
+      <c r="BO60"/>
+      <c r="BP60"/>
+      <c r="BQ60"/>
+      <c r="BR60"/>
+      <c r="BS60"/>
+      <c r="BT60"/>
+      <c r="BU60"/>
+      <c r="BV60"/>
+      <c r="BW60"/>
+      <c r="BX60"/>
+      <c r="BY60"/>
+      <c r="BZ60"/>
+      <c r="CA60"/>
+      <c r="CB60"/>
+      <c r="CC60"/>
+      <c r="CD60"/>
+      <c r="CE60"/>
+      <c r="CF60"/>
+      <c r="CG60"/>
+      <c r="CH60"/>
+      <c r="CI60"/>
+      <c r="CJ60"/>
+      <c r="CK60"/>
+      <c r="CL60"/>
+      <c r="CM60"/>
+      <c r="CN60"/>
+      <c r="CO60"/>
+      <c r="CP60"/>
+      <c r="CQ60"/>
+      <c r="CR60"/>
+      <c r="CS60"/>
+      <c r="CT60"/>
+      <c r="CU60"/>
+      <c r="CV60"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61"/>
+      <c r="Y61"/>
+      <c r="Z61"/>
+      <c r="AA61"/>
+      <c r="AB61"/>
+      <c r="AC61"/>
+      <c r="AD61"/>
+      <c r="AE61"/>
+      <c r="AF61"/>
+      <c r="AG61"/>
+      <c r="AH61"/>
+      <c r="AI61"/>
+      <c r="AJ61"/>
+      <c r="AK61"/>
+      <c r="AL61"/>
+      <c r="AM61"/>
+      <c r="AN61"/>
+      <c r="AO61"/>
+      <c r="AP61"/>
+      <c r="AQ61"/>
+      <c r="AR61"/>
+      <c r="AS61"/>
+      <c r="AT61"/>
+      <c r="AU61"/>
+      <c r="AV61"/>
+      <c r="AW61"/>
+      <c r="AX61"/>
+      <c r="AY61"/>
+      <c r="AZ61"/>
+      <c r="BA61"/>
+      <c r="BB61"/>
+      <c r="BC61"/>
+      <c r="BD61"/>
+      <c r="BE61"/>
+      <c r="BF61"/>
+      <c r="BG61"/>
+      <c r="BH61"/>
+      <c r="BI61"/>
+      <c r="BJ61"/>
+      <c r="BK61"/>
+      <c r="BL61"/>
+      <c r="BM61"/>
+      <c r="BN61"/>
+      <c r="BO61"/>
+      <c r="BP61"/>
+      <c r="BQ61"/>
+      <c r="BR61"/>
+      <c r="BS61"/>
+      <c r="BT61"/>
+      <c r="BU61"/>
+      <c r="BV61"/>
+      <c r="BW61"/>
+      <c r="BX61"/>
+      <c r="BY61"/>
+      <c r="BZ61"/>
+      <c r="CA61"/>
+      <c r="CB61"/>
+      <c r="CC61"/>
+      <c r="CD61"/>
+      <c r="CE61"/>
+      <c r="CF61"/>
+      <c r="CG61"/>
+      <c r="CH61"/>
+      <c r="CI61"/>
+      <c r="CJ61"/>
+      <c r="CK61"/>
+      <c r="CL61"/>
+      <c r="CM61"/>
+      <c r="CN61"/>
+      <c r="CO61"/>
+      <c r="CP61"/>
+      <c r="CQ61"/>
+      <c r="CR61"/>
+      <c r="CS61"/>
+      <c r="CT61"/>
+      <c r="CU61"/>
+      <c r="CV61"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62"/>
+      <c r="Y62"/>
+      <c r="Z62"/>
+      <c r="AA62"/>
+      <c r="AB62"/>
+      <c r="AC62"/>
+      <c r="AD62"/>
+      <c r="AE62"/>
+      <c r="AF62"/>
+      <c r="AG62"/>
+      <c r="AH62"/>
+      <c r="AI62"/>
+      <c r="AJ62"/>
+      <c r="AK62"/>
+      <c r="AL62"/>
+      <c r="AM62"/>
+      <c r="AN62"/>
+      <c r="AO62"/>
+      <c r="AP62"/>
+      <c r="AQ62"/>
+      <c r="AR62"/>
+      <c r="AS62"/>
+      <c r="AT62"/>
+      <c r="AU62"/>
+      <c r="AV62"/>
+      <c r="AW62"/>
+      <c r="AX62"/>
+      <c r="AY62"/>
+      <c r="AZ62"/>
+      <c r="BA62"/>
+      <c r="BB62"/>
+      <c r="BC62"/>
+      <c r="BD62"/>
+      <c r="BE62"/>
+      <c r="BF62"/>
+      <c r="BG62"/>
+      <c r="BH62"/>
+      <c r="BI62"/>
+      <c r="BJ62"/>
+      <c r="BK62"/>
+      <c r="BL62"/>
+      <c r="BM62"/>
+      <c r="BN62"/>
+      <c r="BO62"/>
+      <c r="BP62"/>
+      <c r="BQ62"/>
+      <c r="BR62"/>
+      <c r="BS62"/>
+      <c r="BT62"/>
+      <c r="BU62"/>
+      <c r="BV62"/>
+      <c r="BW62"/>
+      <c r="BX62"/>
+      <c r="BY62"/>
+      <c r="BZ62"/>
+      <c r="CA62"/>
+      <c r="CB62"/>
+      <c r="CC62"/>
+      <c r="CD62"/>
+      <c r="CE62"/>
+      <c r="CF62"/>
+      <c r="CG62"/>
+      <c r="CH62"/>
+      <c r="CI62"/>
+      <c r="CJ62"/>
+      <c r="CK62"/>
+      <c r="CL62"/>
+      <c r="CM62"/>
+      <c r="CN62"/>
+      <c r="CO62"/>
+      <c r="CP62"/>
+      <c r="CQ62"/>
+      <c r="CR62"/>
+      <c r="CS62"/>
+      <c r="CT62"/>
+      <c r="CU62"/>
+      <c r="CV62"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63"/>
+      <c r="Y63"/>
+      <c r="Z63"/>
+      <c r="AA63"/>
+      <c r="AB63"/>
+      <c r="AC63"/>
+      <c r="AD63"/>
+      <c r="AE63"/>
+      <c r="AF63"/>
+      <c r="AG63"/>
+      <c r="AH63"/>
+      <c r="AI63"/>
+      <c r="AJ63"/>
+      <c r="AK63"/>
+      <c r="AL63"/>
+      <c r="AM63"/>
+      <c r="AN63"/>
+      <c r="AO63"/>
+      <c r="AP63"/>
+      <c r="AQ63"/>
+      <c r="AR63"/>
+      <c r="AS63"/>
+      <c r="AT63"/>
+      <c r="AU63"/>
+      <c r="AV63"/>
+      <c r="AW63"/>
+      <c r="AX63"/>
+      <c r="AY63"/>
+      <c r="AZ63"/>
+      <c r="BA63"/>
+      <c r="BB63"/>
+      <c r="BC63"/>
+      <c r="BD63"/>
+      <c r="BE63"/>
+      <c r="BF63"/>
+      <c r="BG63"/>
+      <c r="BH63"/>
+      <c r="BI63"/>
+      <c r="BJ63"/>
+      <c r="BK63"/>
+      <c r="BL63"/>
+      <c r="BM63"/>
+      <c r="BN63"/>
+      <c r="BO63"/>
+      <c r="BP63"/>
+      <c r="BQ63"/>
+      <c r="BR63"/>
+      <c r="BS63"/>
+      <c r="BT63"/>
+      <c r="BU63"/>
+      <c r="BV63"/>
+      <c r="BW63"/>
+      <c r="BX63"/>
+      <c r="BY63"/>
+      <c r="BZ63"/>
+      <c r="CA63"/>
+      <c r="CB63"/>
+      <c r="CC63"/>
+      <c r="CD63"/>
+      <c r="CE63"/>
+      <c r="CF63"/>
+      <c r="CG63"/>
+      <c r="CH63"/>
+      <c r="CI63"/>
+      <c r="CJ63"/>
+      <c r="CK63"/>
+      <c r="CL63"/>
+      <c r="CM63"/>
+      <c r="CN63"/>
+      <c r="CO63"/>
+      <c r="CP63"/>
+      <c r="CQ63"/>
+      <c r="CR63"/>
+      <c r="CS63"/>
+      <c r="CT63"/>
+      <c r="CU63"/>
+      <c r="CV63"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64"/>
+      <c r="Y64"/>
+      <c r="Z64"/>
+      <c r="AA64"/>
+      <c r="AB64"/>
+      <c r="AC64"/>
+      <c r="AD64"/>
+      <c r="AE64"/>
+      <c r="AF64"/>
+      <c r="AG64"/>
+      <c r="AH64"/>
+      <c r="AI64"/>
+      <c r="AJ64"/>
+      <c r="AK64"/>
+      <c r="AL64"/>
+      <c r="AM64"/>
+      <c r="AN64"/>
+      <c r="AO64"/>
+      <c r="AP64"/>
+      <c r="AQ64"/>
+      <c r="AR64"/>
+      <c r="AS64"/>
+      <c r="AT64"/>
+      <c r="AU64"/>
+      <c r="AV64"/>
+      <c r="AW64"/>
+      <c r="AX64"/>
+      <c r="AY64"/>
+      <c r="AZ64"/>
+      <c r="BA64"/>
+      <c r="BB64"/>
+      <c r="BC64"/>
+      <c r="BD64"/>
+      <c r="BE64"/>
+      <c r="BF64"/>
+      <c r="BG64"/>
+      <c r="BH64"/>
+      <c r="BI64"/>
+      <c r="BJ64"/>
+      <c r="BK64"/>
+      <c r="BL64"/>
+      <c r="BM64"/>
+      <c r="BN64"/>
+      <c r="BO64"/>
+      <c r="BP64"/>
+      <c r="BQ64"/>
+      <c r="BR64"/>
+      <c r="BS64"/>
+      <c r="BT64"/>
+      <c r="BU64"/>
+      <c r="BV64"/>
+      <c r="BW64"/>
+      <c r="BX64"/>
+      <c r="BY64"/>
+      <c r="BZ64"/>
+      <c r="CA64"/>
+      <c r="CB64"/>
+      <c r="CC64"/>
+      <c r="CD64"/>
+      <c r="CE64"/>
+      <c r="CF64"/>
+      <c r="CG64"/>
+      <c r="CH64"/>
+      <c r="CI64"/>
+      <c r="CJ64"/>
+      <c r="CK64"/>
+      <c r="CL64"/>
+      <c r="CM64"/>
+      <c r="CN64"/>
+      <c r="CO64"/>
+      <c r="CP64"/>
+      <c r="CQ64"/>
+      <c r="CR64"/>
+      <c r="CS64"/>
+      <c r="CT64"/>
+      <c r="CU64"/>
+      <c r="CV64"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65"/>
+      <c r="Y65"/>
+      <c r="Z65"/>
+      <c r="AA65"/>
+      <c r="AB65"/>
+      <c r="AC65"/>
+      <c r="AD65"/>
+      <c r="AE65"/>
+      <c r="AF65"/>
+      <c r="AG65"/>
+      <c r="AH65"/>
+      <c r="AI65"/>
+      <c r="AJ65"/>
+      <c r="AK65"/>
+      <c r="AL65"/>
+      <c r="AM65"/>
+      <c r="AN65"/>
+      <c r="AO65"/>
+      <c r="AP65"/>
+      <c r="AQ65"/>
+      <c r="AR65"/>
+      <c r="AS65"/>
+      <c r="AT65"/>
+      <c r="AU65"/>
+      <c r="AV65"/>
+      <c r="AW65"/>
+      <c r="AX65"/>
+      <c r="AY65"/>
+      <c r="AZ65"/>
+      <c r="BA65"/>
+      <c r="BB65"/>
+      <c r="BC65"/>
+      <c r="BD65"/>
+      <c r="BE65"/>
+      <c r="BF65"/>
+      <c r="BG65"/>
+      <c r="BH65"/>
+      <c r="BI65"/>
+      <c r="BJ65"/>
+      <c r="BK65"/>
+      <c r="BL65"/>
+      <c r="BM65"/>
+      <c r="BN65"/>
+      <c r="BO65"/>
+      <c r="BP65"/>
+      <c r="BQ65"/>
+      <c r="BR65"/>
+      <c r="BS65"/>
+      <c r="BT65"/>
+      <c r="BU65"/>
+      <c r="BV65"/>
+      <c r="BW65"/>
+      <c r="BX65"/>
+      <c r="BY65"/>
+      <c r="BZ65"/>
+      <c r="CA65"/>
+      <c r="CB65"/>
+      <c r="CC65"/>
+      <c r="CD65"/>
+      <c r="CE65"/>
+      <c r="CF65"/>
+      <c r="CG65"/>
+      <c r="CH65"/>
+      <c r="CI65"/>
+      <c r="CJ65"/>
+      <c r="CK65"/>
+      <c r="CL65"/>
+      <c r="CM65"/>
+      <c r="CN65"/>
+      <c r="CO65"/>
+      <c r="CP65"/>
+      <c r="CQ65"/>
+      <c r="CR65"/>
+      <c r="CS65"/>
+      <c r="CT65"/>
+      <c r="CU65"/>
+      <c r="CV65"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+      <c r="Y66"/>
+      <c r="Z66"/>
+      <c r="AA66"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
+      <c r="AD66"/>
+      <c r="AE66"/>
+      <c r="AF66"/>
+      <c r="AG66"/>
+      <c r="AH66"/>
+      <c r="AI66"/>
+      <c r="AJ66"/>
+      <c r="AK66"/>
+      <c r="AL66"/>
+      <c r="AM66"/>
+      <c r="AN66"/>
+      <c r="AO66"/>
+      <c r="AP66"/>
+      <c r="AQ66"/>
+      <c r="AR66"/>
+      <c r="AS66"/>
+      <c r="AT66"/>
+      <c r="AU66"/>
+      <c r="AV66"/>
+      <c r="AW66"/>
+      <c r="AX66"/>
+      <c r="AY66"/>
+      <c r="AZ66"/>
+      <c r="BA66"/>
+      <c r="BB66"/>
+      <c r="BC66"/>
+      <c r="BD66"/>
+      <c r="BE66"/>
+      <c r="BF66"/>
+      <c r="BG66"/>
+      <c r="BH66"/>
+      <c r="BI66"/>
+      <c r="BJ66"/>
+      <c r="BK66"/>
+      <c r="BL66"/>
+      <c r="BM66"/>
+      <c r="BN66"/>
+      <c r="BO66"/>
+      <c r="BP66"/>
+      <c r="BQ66"/>
+      <c r="BR66"/>
+      <c r="BS66"/>
+      <c r="BT66"/>
+      <c r="BU66"/>
+      <c r="BV66"/>
+      <c r="BW66"/>
+      <c r="BX66"/>
+      <c r="BY66"/>
+      <c r="BZ66"/>
+      <c r="CA66"/>
+      <c r="CB66"/>
+      <c r="CC66"/>
+      <c r="CD66"/>
+      <c r="CE66"/>
+      <c r="CF66"/>
+      <c r="CG66"/>
+      <c r="CH66"/>
+      <c r="CI66"/>
+      <c r="CJ66"/>
+      <c r="CK66"/>
+      <c r="CL66"/>
+      <c r="CM66"/>
+      <c r="CN66"/>
+      <c r="CO66"/>
+      <c r="CP66"/>
+      <c r="CQ66"/>
+      <c r="CR66"/>
+      <c r="CS66"/>
+      <c r="CT66"/>
+      <c r="CU66"/>
+      <c r="CV66"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+      <c r="AE67"/>
+      <c r="AF67"/>
+      <c r="AG67"/>
+      <c r="AH67"/>
+      <c r="AI67"/>
+      <c r="AJ67"/>
+      <c r="AK67"/>
+      <c r="AL67"/>
+      <c r="AM67"/>
+      <c r="AN67"/>
+      <c r="AO67"/>
+      <c r="AP67"/>
+      <c r="AQ67"/>
+      <c r="AR67"/>
+      <c r="AS67"/>
+      <c r="AT67"/>
+      <c r="AU67"/>
+      <c r="AV67"/>
+      <c r="AW67"/>
+      <c r="AX67"/>
+      <c r="AY67"/>
+      <c r="AZ67"/>
+      <c r="BA67"/>
+      <c r="BB67"/>
+      <c r="BC67"/>
+      <c r="BD67"/>
+      <c r="BE67"/>
+      <c r="BF67"/>
+      <c r="BG67"/>
+      <c r="BH67"/>
+      <c r="BI67"/>
+      <c r="BJ67"/>
+      <c r="BK67"/>
+      <c r="BL67"/>
+      <c r="BM67"/>
+      <c r="BN67"/>
+      <c r="BO67"/>
+      <c r="BP67"/>
+      <c r="BQ67"/>
+      <c r="BR67"/>
+      <c r="BS67"/>
+      <c r="BT67"/>
+      <c r="BU67"/>
+      <c r="BV67"/>
+      <c r="BW67"/>
+      <c r="BX67"/>
+      <c r="BY67"/>
+      <c r="BZ67"/>
+      <c r="CA67"/>
+      <c r="CB67"/>
+      <c r="CC67"/>
+      <c r="CD67"/>
+      <c r="CE67"/>
+      <c r="CF67"/>
+      <c r="CG67"/>
+      <c r="CH67"/>
+      <c r="CI67"/>
+      <c r="CJ67"/>
+      <c r="CK67"/>
+      <c r="CL67"/>
+      <c r="CM67"/>
+      <c r="CN67"/>
+      <c r="CO67"/>
+      <c r="CP67"/>
+      <c r="CQ67"/>
+      <c r="CR67"/>
+      <c r="CS67"/>
+      <c r="CT67"/>
+      <c r="CU67"/>
+      <c r="CV67"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+      <c r="Z68"/>
+      <c r="AA68"/>
+      <c r="AB68"/>
+      <c r="AC68"/>
+      <c r="AD68"/>
+      <c r="AE68"/>
+      <c r="AF68"/>
+      <c r="AG68"/>
+      <c r="AH68"/>
+      <c r="AI68"/>
+      <c r="AJ68"/>
+      <c r="AK68"/>
+      <c r="AL68"/>
+      <c r="AM68"/>
+      <c r="AN68"/>
+      <c r="AO68"/>
+      <c r="AP68"/>
+      <c r="AQ68"/>
+      <c r="AR68"/>
+      <c r="AS68"/>
+      <c r="AT68"/>
+      <c r="AU68"/>
+      <c r="AV68"/>
+      <c r="AW68"/>
+      <c r="AX68"/>
+      <c r="AY68"/>
+      <c r="AZ68"/>
+      <c r="BA68"/>
+      <c r="BB68"/>
+      <c r="BC68"/>
+      <c r="BD68"/>
+      <c r="BE68"/>
+      <c r="BF68"/>
+      <c r="BG68"/>
+      <c r="BH68"/>
+      <c r="BI68"/>
+      <c r="BJ68"/>
+      <c r="BK68"/>
+      <c r="BL68"/>
+      <c r="BM68"/>
+      <c r="BN68"/>
+      <c r="BO68"/>
+      <c r="BP68"/>
+      <c r="BQ68"/>
+      <c r="BR68"/>
+      <c r="BS68"/>
+      <c r="BT68"/>
+      <c r="BU68"/>
+      <c r="BV68"/>
+      <c r="BW68"/>
+      <c r="BX68"/>
+      <c r="BY68"/>
+      <c r="BZ68"/>
+      <c r="CA68"/>
+      <c r="CB68"/>
+      <c r="CC68"/>
+      <c r="CD68"/>
+      <c r="CE68"/>
+      <c r="CF68"/>
+      <c r="CG68"/>
+      <c r="CH68"/>
+      <c r="CI68"/>
+      <c r="CJ68"/>
+      <c r="CK68"/>
+      <c r="CL68"/>
+      <c r="CM68"/>
+      <c r="CN68"/>
+      <c r="CO68"/>
+      <c r="CP68"/>
+      <c r="CQ68"/>
+      <c r="CR68"/>
+      <c r="CS68"/>
+      <c r="CT68"/>
+      <c r="CU68"/>
+      <c r="CV68"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+      <c r="U69"/>
+      <c r="V69"/>
+      <c r="W69"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+      <c r="AA69"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
+      <c r="AE69"/>
+      <c r="AF69"/>
+      <c r="AG69"/>
+      <c r="AH69"/>
+      <c r="AI69"/>
+      <c r="AJ69"/>
+      <c r="AK69"/>
+      <c r="AL69"/>
+      <c r="AM69"/>
+      <c r="AN69"/>
+      <c r="AO69"/>
+      <c r="AP69"/>
+      <c r="AQ69"/>
+      <c r="AR69"/>
+      <c r="AS69"/>
+      <c r="AT69"/>
+      <c r="AU69"/>
+      <c r="AV69"/>
+      <c r="AW69"/>
+      <c r="AX69"/>
+      <c r="AY69"/>
+      <c r="AZ69"/>
+      <c r="BA69"/>
+      <c r="BB69"/>
+      <c r="BC69"/>
+      <c r="BD69"/>
+      <c r="BE69"/>
+      <c r="BF69"/>
+      <c r="BG69"/>
+      <c r="BH69"/>
+      <c r="BI69"/>
+      <c r="BJ69"/>
+      <c r="BK69"/>
+      <c r="BL69"/>
+      <c r="BM69"/>
+      <c r="BN69"/>
+      <c r="BO69"/>
+      <c r="BP69"/>
+      <c r="BQ69"/>
+      <c r="BR69"/>
+      <c r="BS69"/>
+      <c r="BT69"/>
+      <c r="BU69"/>
+      <c r="BV69"/>
+      <c r="BW69"/>
+      <c r="BX69"/>
+      <c r="BY69"/>
+      <c r="BZ69"/>
+      <c r="CA69"/>
+      <c r="CB69"/>
+      <c r="CC69"/>
+      <c r="CD69"/>
+      <c r="CE69"/>
+      <c r="CF69"/>
+      <c r="CG69"/>
+      <c r="CH69"/>
+      <c r="CI69"/>
+      <c r="CJ69"/>
+      <c r="CK69"/>
+      <c r="CL69"/>
+      <c r="CM69"/>
+      <c r="CN69"/>
+      <c r="CO69"/>
+      <c r="CP69"/>
+      <c r="CQ69"/>
+      <c r="CR69"/>
+      <c r="CS69"/>
+      <c r="CT69"/>
+      <c r="CU69"/>
+      <c r="CV69"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70"/>
+      <c r="T70"/>
+      <c r="U70"/>
+      <c r="V70"/>
+      <c r="W70"/>
+      <c r="X70"/>
+      <c r="Y70"/>
+      <c r="Z70"/>
+      <c r="AA70"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
+      <c r="AD70"/>
+      <c r="AE70"/>
+      <c r="AF70"/>
+      <c r="AG70"/>
+      <c r="AH70"/>
+      <c r="AI70"/>
+      <c r="AJ70"/>
+      <c r="AK70"/>
+      <c r="AL70"/>
+      <c r="AM70"/>
+      <c r="AN70"/>
+      <c r="AO70"/>
+      <c r="AP70"/>
+      <c r="AQ70"/>
+      <c r="AR70"/>
+      <c r="AS70"/>
+      <c r="AT70"/>
+      <c r="AU70"/>
+      <c r="AV70"/>
+      <c r="AW70"/>
+      <c r="AX70"/>
+      <c r="AY70"/>
+      <c r="AZ70"/>
+      <c r="BA70"/>
+      <c r="BB70"/>
+      <c r="BC70"/>
+      <c r="BD70"/>
+      <c r="BE70"/>
+      <c r="BF70"/>
+      <c r="BG70"/>
+      <c r="BH70"/>
+      <c r="BI70"/>
+      <c r="BJ70"/>
+      <c r="BK70"/>
+      <c r="BL70"/>
+      <c r="BM70"/>
+      <c r="BN70"/>
+      <c r="BO70"/>
+      <c r="BP70"/>
+      <c r="BQ70"/>
+      <c r="BR70"/>
+      <c r="BS70"/>
+      <c r="BT70"/>
+      <c r="BU70"/>
+      <c r="BV70"/>
+      <c r="BW70"/>
+      <c r="BX70"/>
+      <c r="BY70"/>
+      <c r="BZ70"/>
+      <c r="CA70"/>
+      <c r="CB70"/>
+      <c r="CC70"/>
+      <c r="CD70"/>
+      <c r="CE70"/>
+      <c r="CF70"/>
+      <c r="CG70"/>
+      <c r="CH70"/>
+      <c r="CI70"/>
+      <c r="CJ70"/>
+      <c r="CK70"/>
+      <c r="CL70"/>
+      <c r="CM70"/>
+      <c r="CN70"/>
+      <c r="CO70"/>
+      <c r="CP70"/>
+      <c r="CQ70"/>
+      <c r="CR70"/>
+      <c r="CS70"/>
+      <c r="CT70"/>
+      <c r="CU70"/>
+      <c r="CV70"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71"/>
+      <c r="Y71"/>
+      <c r="Z71"/>
+      <c r="AA71"/>
+      <c r="AB71"/>
+      <c r="AC71"/>
+      <c r="AD71"/>
+      <c r="AE71"/>
+      <c r="AF71"/>
+      <c r="AG71"/>
+      <c r="AH71"/>
+      <c r="AI71"/>
+      <c r="AJ71"/>
+      <c r="AK71"/>
+      <c r="AL71"/>
+      <c r="AM71"/>
+      <c r="AN71"/>
+      <c r="AO71"/>
+      <c r="AP71"/>
+      <c r="AQ71"/>
+      <c r="AR71"/>
+      <c r="AS71"/>
+      <c r="AT71"/>
+      <c r="AU71"/>
+      <c r="AV71"/>
+      <c r="AW71"/>
+      <c r="AX71"/>
+      <c r="AY71"/>
+      <c r="AZ71"/>
+      <c r="BA71"/>
+      <c r="BB71"/>
+      <c r="BC71"/>
+      <c r="BD71"/>
+      <c r="BE71"/>
+      <c r="BF71"/>
+      <c r="BG71"/>
+      <c r="BH71"/>
+      <c r="BI71"/>
+      <c r="BJ71"/>
+      <c r="BK71"/>
+      <c r="BL71"/>
+      <c r="BM71"/>
+      <c r="BN71"/>
+      <c r="BO71"/>
+      <c r="BP71"/>
+      <c r="BQ71"/>
+      <c r="BR71"/>
+      <c r="BS71"/>
+      <c r="BT71"/>
+      <c r="BU71"/>
+      <c r="BV71"/>
+      <c r="BW71"/>
+      <c r="BX71"/>
+      <c r="BY71"/>
+      <c r="BZ71"/>
+      <c r="CA71"/>
+      <c r="CB71"/>
+      <c r="CC71"/>
+      <c r="CD71"/>
+      <c r="CE71"/>
+      <c r="CF71"/>
+      <c r="CG71"/>
+      <c r="CH71"/>
+      <c r="CI71"/>
+      <c r="CJ71"/>
+      <c r="CK71"/>
+      <c r="CL71"/>
+      <c r="CM71"/>
+      <c r="CN71"/>
+      <c r="CO71"/>
+      <c r="CP71"/>
+      <c r="CQ71"/>
+      <c r="CR71"/>
+      <c r="CS71"/>
+      <c r="CT71"/>
+      <c r="CU71"/>
+      <c r="CV71"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+      <c r="U72"/>
+      <c r="V72"/>
+      <c r="W72"/>
+      <c r="X72"/>
+      <c r="Y72"/>
+      <c r="Z72"/>
+      <c r="AA72"/>
+      <c r="AB72"/>
+      <c r="AC72"/>
+      <c r="AD72"/>
+      <c r="AE72"/>
+      <c r="AF72"/>
+      <c r="AG72"/>
+      <c r="AH72"/>
+      <c r="AI72"/>
+      <c r="AJ72"/>
+      <c r="AK72"/>
+      <c r="AL72"/>
+      <c r="AM72"/>
+      <c r="AN72"/>
+      <c r="AO72"/>
+      <c r="AP72"/>
+      <c r="AQ72"/>
+      <c r="AR72"/>
+      <c r="AS72"/>
+      <c r="AT72"/>
+      <c r="AU72"/>
+      <c r="AV72"/>
+      <c r="AW72"/>
+      <c r="AX72"/>
+      <c r="AY72"/>
+      <c r="AZ72"/>
+      <c r="BA72"/>
+      <c r="BB72"/>
+      <c r="BC72"/>
+      <c r="BD72"/>
+      <c r="BE72"/>
+      <c r="BF72"/>
+      <c r="BG72"/>
+      <c r="BH72"/>
+      <c r="BI72"/>
+      <c r="BJ72"/>
+      <c r="BK72"/>
+      <c r="BL72"/>
+      <c r="BM72"/>
+      <c r="BN72"/>
+      <c r="BO72"/>
+      <c r="BP72"/>
+      <c r="BQ72"/>
+      <c r="BR72"/>
+      <c r="BS72"/>
+      <c r="BT72"/>
+      <c r="BU72"/>
+      <c r="BV72"/>
+      <c r="BW72"/>
+      <c r="BX72"/>
+      <c r="BY72"/>
+      <c r="BZ72"/>
+      <c r="CA72"/>
+      <c r="CB72"/>
+      <c r="CC72"/>
+      <c r="CD72"/>
+      <c r="CE72"/>
+      <c r="CF72"/>
+      <c r="CG72"/>
+      <c r="CH72"/>
+      <c r="CI72"/>
+      <c r="CJ72"/>
+      <c r="CK72"/>
+      <c r="CL72"/>
+      <c r="CM72"/>
+      <c r="CN72"/>
+      <c r="CO72"/>
+      <c r="CP72"/>
+      <c r="CQ72"/>
+      <c r="CR72"/>
+      <c r="CS72"/>
+      <c r="CT72"/>
+      <c r="CU72"/>
+      <c r="CV72"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+      <c r="V73"/>
+      <c r="W73"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+      <c r="AE73"/>
+      <c r="AF73"/>
+      <c r="AG73"/>
+      <c r="AH73"/>
+      <c r="AI73"/>
+      <c r="AJ73"/>
+      <c r="AK73"/>
+      <c r="AL73"/>
+      <c r="AM73"/>
+      <c r="AN73"/>
+      <c r="AO73"/>
+      <c r="AP73"/>
+      <c r="AQ73"/>
+      <c r="AR73"/>
+      <c r="AS73"/>
+      <c r="AT73"/>
+      <c r="AU73"/>
+      <c r="AV73"/>
+      <c r="AW73"/>
+      <c r="AX73"/>
+      <c r="AY73"/>
+      <c r="AZ73"/>
+      <c r="BA73"/>
+      <c r="BB73"/>
+      <c r="BC73"/>
+      <c r="BD73"/>
+      <c r="BE73"/>
+      <c r="BF73"/>
+      <c r="BG73"/>
+      <c r="BH73"/>
+      <c r="BI73"/>
+      <c r="BJ73"/>
+      <c r="BK73"/>
+      <c r="BL73"/>
+      <c r="BM73"/>
+      <c r="BN73"/>
+      <c r="BO73"/>
+      <c r="BP73"/>
+      <c r="BQ73"/>
+      <c r="BR73"/>
+      <c r="BS73"/>
+      <c r="BT73"/>
+      <c r="BU73"/>
+      <c r="BV73"/>
+      <c r="BW73"/>
+      <c r="BX73"/>
+      <c r="BY73"/>
+      <c r="BZ73"/>
+      <c r="CA73"/>
+      <c r="CB73"/>
+      <c r="CC73"/>
+      <c r="CD73"/>
+      <c r="CE73"/>
+      <c r="CF73"/>
+      <c r="CG73"/>
+      <c r="CH73"/>
+      <c r="CI73"/>
+      <c r="CJ73"/>
+      <c r="CK73"/>
+      <c r="CL73"/>
+      <c r="CM73"/>
+      <c r="CN73"/>
+      <c r="CO73"/>
+      <c r="CP73"/>
+      <c r="CQ73"/>
+      <c r="CR73"/>
+      <c r="CS73"/>
+      <c r="CT73"/>
+      <c r="CU73"/>
+      <c r="CV73"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+      <c r="T74"/>
+      <c r="U74"/>
+      <c r="V74"/>
+      <c r="W74"/>
+      <c r="X74"/>
+      <c r="Y74"/>
+      <c r="Z74"/>
+      <c r="AA74"/>
+      <c r="AB74"/>
+      <c r="AC74"/>
+      <c r="AD74"/>
+      <c r="AE74"/>
+      <c r="AF74"/>
+      <c r="AG74"/>
+      <c r="AH74"/>
+      <c r="AI74"/>
+      <c r="AJ74"/>
+      <c r="AK74"/>
+      <c r="AL74"/>
+      <c r="AM74"/>
+      <c r="AN74"/>
+      <c r="AO74"/>
+      <c r="AP74"/>
+      <c r="AQ74"/>
+      <c r="AR74"/>
+      <c r="AS74"/>
+      <c r="AT74"/>
+      <c r="AU74"/>
+      <c r="AV74"/>
+      <c r="AW74"/>
+      <c r="AX74"/>
+      <c r="AY74"/>
+      <c r="AZ74"/>
+      <c r="BA74"/>
+      <c r="BB74"/>
+      <c r="BC74"/>
+      <c r="BD74"/>
+      <c r="BE74"/>
+      <c r="BF74"/>
+      <c r="BG74"/>
+      <c r="BH74"/>
+      <c r="BI74"/>
+      <c r="BJ74"/>
+      <c r="BK74"/>
+      <c r="BL74"/>
+      <c r="BM74"/>
+      <c r="BN74"/>
+      <c r="BO74"/>
+      <c r="BP74"/>
+      <c r="BQ74"/>
+      <c r="BR74"/>
+      <c r="BS74"/>
+      <c r="BT74"/>
+      <c r="BU74"/>
+      <c r="BV74"/>
+      <c r="BW74"/>
+      <c r="BX74"/>
+      <c r="BY74"/>
+      <c r="BZ74"/>
+      <c r="CA74"/>
+      <c r="CB74"/>
+      <c r="CC74"/>
+      <c r="CD74"/>
+      <c r="CE74"/>
+      <c r="CF74"/>
+      <c r="CG74"/>
+      <c r="CH74"/>
+      <c r="CI74"/>
+      <c r="CJ74"/>
+      <c r="CK74"/>
+      <c r="CL74"/>
+      <c r="CM74"/>
+      <c r="CN74"/>
+      <c r="CO74"/>
+      <c r="CP74"/>
+      <c r="CQ74"/>
+      <c r="CR74"/>
+      <c r="CS74"/>
+      <c r="CT74"/>
+      <c r="CU74"/>
+      <c r="CV74"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+      <c r="R75"/>
+      <c r="S75"/>
+      <c r="T75"/>
+      <c r="U75"/>
+      <c r="V75"/>
+      <c r="W75"/>
+      <c r="X75"/>
+      <c r="Y75"/>
+      <c r="Z75"/>
+      <c r="AA75"/>
+      <c r="AB75"/>
+      <c r="AC75"/>
+      <c r="AD75"/>
+      <c r="AE75"/>
+      <c r="AF75"/>
+      <c r="AG75"/>
+      <c r="AH75"/>
+      <c r="AI75"/>
+      <c r="AJ75"/>
+      <c r="AK75"/>
+      <c r="AL75"/>
+      <c r="AM75"/>
+      <c r="AN75"/>
+      <c r="AO75"/>
+      <c r="AP75"/>
+      <c r="AQ75"/>
+      <c r="AR75"/>
+      <c r="AS75"/>
+      <c r="AT75"/>
+      <c r="AU75"/>
+      <c r="AV75"/>
+      <c r="AW75"/>
+      <c r="AX75"/>
+      <c r="AY75"/>
+      <c r="AZ75"/>
+      <c r="BA75"/>
+      <c r="BB75"/>
+      <c r="BC75"/>
+      <c r="BD75"/>
+      <c r="BE75"/>
+      <c r="BF75"/>
+      <c r="BG75"/>
+      <c r="BH75"/>
+      <c r="BI75"/>
+      <c r="BJ75"/>
+      <c r="BK75"/>
+      <c r="BL75"/>
+      <c r="BM75"/>
+      <c r="BN75"/>
+      <c r="BO75"/>
+      <c r="BP75"/>
+      <c r="BQ75"/>
+      <c r="BR75"/>
+      <c r="BS75"/>
+      <c r="BT75"/>
+      <c r="BU75"/>
+      <c r="BV75"/>
+      <c r="BW75"/>
+      <c r="BX75"/>
+      <c r="BY75"/>
+      <c r="BZ75"/>
+      <c r="CA75"/>
+      <c r="CB75"/>
+      <c r="CC75"/>
+      <c r="CD75"/>
+      <c r="CE75"/>
+      <c r="CF75"/>
+      <c r="CG75"/>
+      <c r="CH75"/>
+      <c r="CI75"/>
+      <c r="CJ75"/>
+      <c r="CK75"/>
+      <c r="CL75"/>
+      <c r="CM75"/>
+      <c r="CN75"/>
+      <c r="CO75"/>
+      <c r="CP75"/>
+      <c r="CQ75"/>
+      <c r="CR75"/>
+      <c r="CS75"/>
+      <c r="CT75"/>
+      <c r="CU75"/>
+      <c r="CV75"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76"/>
+      <c r="O76"/>
+      <c r="P76"/>
+      <c r="Q76"/>
+      <c r="R76"/>
+      <c r="S76"/>
+      <c r="T76"/>
+      <c r="U76"/>
+      <c r="V76"/>
+      <c r="W76"/>
+      <c r="X76"/>
+      <c r="Y76"/>
+      <c r="Z76"/>
+      <c r="AA76"/>
+      <c r="AB76"/>
+      <c r="AC76"/>
+      <c r="AD76"/>
+      <c r="AE76"/>
+      <c r="AF76"/>
+      <c r="AG76"/>
+      <c r="AH76"/>
+      <c r="AI76"/>
+      <c r="AJ76"/>
+      <c r="AK76"/>
+      <c r="AL76"/>
+      <c r="AM76"/>
+      <c r="AN76"/>
+      <c r="AO76"/>
+      <c r="AP76"/>
+      <c r="AQ76"/>
+      <c r="AR76"/>
+      <c r="AS76"/>
+      <c r="AT76"/>
+      <c r="AU76"/>
+      <c r="AV76"/>
+      <c r="AW76"/>
+      <c r="AX76"/>
+      <c r="AY76"/>
+      <c r="AZ76"/>
+      <c r="BA76"/>
+      <c r="BB76"/>
+      <c r="BC76"/>
+      <c r="BD76"/>
+      <c r="BE76"/>
+      <c r="BF76"/>
+      <c r="BG76"/>
+      <c r="BH76"/>
+      <c r="BI76"/>
+      <c r="BJ76"/>
+      <c r="BK76"/>
+      <c r="BL76"/>
+      <c r="BM76"/>
+      <c r="BN76"/>
+      <c r="BO76"/>
+      <c r="BP76"/>
+      <c r="BQ76"/>
+      <c r="BR76"/>
+      <c r="BS76"/>
+      <c r="BT76"/>
+      <c r="BU76"/>
+      <c r="BV76"/>
+      <c r="BW76"/>
+      <c r="BX76"/>
+      <c r="BY76"/>
+      <c r="BZ76"/>
+      <c r="CA76"/>
+      <c r="CB76"/>
+      <c r="CC76"/>
+      <c r="CD76"/>
+      <c r="CE76"/>
+      <c r="CF76"/>
+      <c r="CG76"/>
+      <c r="CH76"/>
+      <c r="CI76"/>
+      <c r="CJ76"/>
+      <c r="CK76"/>
+      <c r="CL76"/>
+      <c r="CM76"/>
+      <c r="CN76"/>
+      <c r="CO76"/>
+      <c r="CP76"/>
+      <c r="CQ76"/>
+      <c r="CR76"/>
+      <c r="CS76"/>
+      <c r="CT76"/>
+      <c r="CU76"/>
+      <c r="CV76"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77"/>
+      <c r="O77"/>
+      <c r="P77"/>
+      <c r="Q77"/>
+      <c r="R77"/>
+      <c r="S77"/>
+      <c r="T77"/>
+      <c r="U77"/>
+      <c r="V77"/>
+      <c r="W77"/>
+      <c r="X77"/>
+      <c r="Y77"/>
+      <c r="Z77"/>
+      <c r="AA77"/>
+      <c r="AB77"/>
+      <c r="AC77"/>
+      <c r="AD77"/>
+      <c r="AE77"/>
+      <c r="AF77"/>
+      <c r="AG77"/>
+      <c r="AH77"/>
+      <c r="AI77"/>
+      <c r="AJ77"/>
+      <c r="AK77"/>
+      <c r="AL77"/>
+      <c r="AM77"/>
+      <c r="AN77"/>
+      <c r="AO77"/>
+      <c r="AP77"/>
+      <c r="AQ77"/>
+      <c r="AR77"/>
+      <c r="AS77"/>
+      <c r="AT77"/>
+      <c r="AU77"/>
+      <c r="AV77"/>
+      <c r="AW77"/>
+      <c r="AX77"/>
+      <c r="AY77"/>
+      <c r="AZ77"/>
+      <c r="BA77"/>
+      <c r="BB77"/>
+      <c r="BC77"/>
+      <c r="BD77"/>
+      <c r="BE77"/>
+      <c r="BF77"/>
+      <c r="BG77"/>
+      <c r="BH77"/>
+      <c r="BI77"/>
+      <c r="BJ77"/>
+      <c r="BK77"/>
+      <c r="BL77"/>
+      <c r="BM77"/>
+      <c r="BN77"/>
+      <c r="BO77"/>
+      <c r="BP77"/>
+      <c r="BQ77"/>
+      <c r="BR77"/>
+      <c r="BS77"/>
+      <c r="BT77"/>
+      <c r="BU77"/>
+      <c r="BV77"/>
+      <c r="BW77"/>
+      <c r="BX77"/>
+      <c r="BY77"/>
+      <c r="BZ77"/>
+      <c r="CA77"/>
+      <c r="CB77"/>
+      <c r="CC77"/>
+      <c r="CD77"/>
+      <c r="CE77"/>
+      <c r="CF77"/>
+      <c r="CG77"/>
+      <c r="CH77"/>
+      <c r="CI77"/>
+      <c r="CJ77"/>
+      <c r="CK77"/>
+      <c r="CL77"/>
+      <c r="CM77"/>
+      <c r="CN77"/>
+      <c r="CO77"/>
+      <c r="CP77"/>
+      <c r="CQ77"/>
+      <c r="CR77"/>
+      <c r="CS77"/>
+      <c r="CT77"/>
+      <c r="CU77"/>
+      <c r="CV77"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
+      <c r="R78"/>
+      <c r="S78"/>
+      <c r="T78"/>
+      <c r="U78"/>
+      <c r="V78"/>
+      <c r="W78"/>
+      <c r="X78"/>
+      <c r="Y78"/>
+      <c r="Z78"/>
+      <c r="AA78"/>
+      <c r="AB78"/>
+      <c r="AC78"/>
+      <c r="AD78"/>
+      <c r="AE78"/>
+      <c r="AF78"/>
+      <c r="AG78"/>
+      <c r="AH78"/>
+      <c r="AI78"/>
+      <c r="AJ78"/>
+      <c r="AK78"/>
+      <c r="AL78"/>
+      <c r="AM78"/>
+      <c r="AN78"/>
+      <c r="AO78"/>
+      <c r="AP78"/>
+      <c r="AQ78"/>
+      <c r="AR78"/>
+      <c r="AS78"/>
+      <c r="AT78"/>
+      <c r="AU78"/>
+      <c r="AV78"/>
+      <c r="AW78"/>
+      <c r="AX78"/>
+      <c r="AY78"/>
+      <c r="AZ78"/>
+      <c r="BA78"/>
+      <c r="BB78"/>
+      <c r="BC78"/>
+      <c r="BD78"/>
+      <c r="BE78"/>
+      <c r="BF78"/>
+      <c r="BG78"/>
+      <c r="BH78"/>
+      <c r="BI78"/>
+      <c r="BJ78"/>
+      <c r="BK78"/>
+      <c r="BL78"/>
+      <c r="BM78"/>
+      <c r="BN78"/>
+      <c r="BO78"/>
+      <c r="BP78"/>
+      <c r="BQ78"/>
+      <c r="BR78"/>
+      <c r="BS78"/>
+      <c r="BT78"/>
+      <c r="BU78"/>
+      <c r="BV78"/>
+      <c r="BW78"/>
+      <c r="BX78"/>
+      <c r="BY78"/>
+      <c r="BZ78"/>
+      <c r="CA78"/>
+      <c r="CB78"/>
+      <c r="CC78"/>
+      <c r="CD78"/>
+      <c r="CE78"/>
+      <c r="CF78"/>
+      <c r="CG78"/>
+      <c r="CH78"/>
+      <c r="CI78"/>
+      <c r="CJ78"/>
+      <c r="CK78"/>
+      <c r="CL78"/>
+      <c r="CM78"/>
+      <c r="CN78"/>
+      <c r="CO78"/>
+      <c r="CP78"/>
+      <c r="CQ78"/>
+      <c r="CR78"/>
+      <c r="CS78"/>
+      <c r="CT78"/>
+      <c r="CU78"/>
+      <c r="CV78"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79"/>
+      <c r="O79"/>
+      <c r="P79"/>
+      <c r="Q79"/>
+      <c r="R79"/>
+      <c r="S79"/>
+      <c r="T79"/>
+      <c r="U79"/>
+      <c r="V79"/>
+      <c r="W79"/>
+      <c r="X79"/>
+      <c r="Y79"/>
+      <c r="Z79"/>
+      <c r="AA79"/>
+      <c r="AB79"/>
+      <c r="AC79"/>
+      <c r="AD79"/>
+      <c r="AE79"/>
+      <c r="AF79"/>
+      <c r="AG79"/>
+      <c r="AH79"/>
+      <c r="AI79"/>
+      <c r="AJ79"/>
+      <c r="AK79"/>
+      <c r="AL79"/>
+      <c r="AM79"/>
+      <c r="AN79"/>
+      <c r="AO79"/>
+      <c r="AP79"/>
+      <c r="AQ79"/>
+      <c r="AR79"/>
+      <c r="AS79"/>
+      <c r="AT79"/>
+      <c r="AU79"/>
+      <c r="AV79"/>
+      <c r="AW79"/>
+      <c r="AX79"/>
+      <c r="AY79"/>
+      <c r="AZ79"/>
+      <c r="BA79"/>
+      <c r="BB79"/>
+      <c r="BC79"/>
+      <c r="BD79"/>
+      <c r="BE79"/>
+      <c r="BF79"/>
+      <c r="BG79"/>
+      <c r="BH79"/>
+      <c r="BI79"/>
+      <c r="BJ79"/>
+      <c r="BK79"/>
+      <c r="BL79"/>
+      <c r="BM79"/>
+      <c r="BN79"/>
+      <c r="BO79"/>
+      <c r="BP79"/>
+      <c r="BQ79"/>
+      <c r="BR79"/>
+      <c r="BS79"/>
+      <c r="BT79"/>
+      <c r="BU79"/>
+      <c r="BV79"/>
+      <c r="BW79"/>
+      <c r="BX79"/>
+      <c r="BY79"/>
+      <c r="BZ79"/>
+      <c r="CA79"/>
+      <c r="CB79"/>
+      <c r="CC79"/>
+      <c r="CD79"/>
+      <c r="CE79"/>
+      <c r="CF79"/>
+      <c r="CG79"/>
+      <c r="CH79"/>
+      <c r="CI79"/>
+      <c r="CJ79"/>
+      <c r="CK79"/>
+      <c r="CL79"/>
+      <c r="CM79"/>
+      <c r="CN79"/>
+      <c r="CO79"/>
+      <c r="CP79"/>
+      <c r="CQ79"/>
+      <c r="CR79"/>
+      <c r="CS79"/>
+      <c r="CT79"/>
+      <c r="CU79"/>
+      <c r="CV79"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
+      <c r="R80"/>
+      <c r="S80"/>
+      <c r="T80"/>
+      <c r="U80"/>
+      <c r="V80"/>
+      <c r="W80"/>
+      <c r="X80"/>
+      <c r="Y80"/>
+      <c r="Z80"/>
+      <c r="AA80"/>
+      <c r="AB80"/>
+      <c r="AC80"/>
+      <c r="AD80"/>
+      <c r="AE80"/>
+      <c r="AF80"/>
+      <c r="AG80"/>
+      <c r="AH80"/>
+      <c r="AI80"/>
+      <c r="AJ80"/>
+      <c r="AK80"/>
+      <c r="AL80"/>
+      <c r="AM80"/>
+      <c r="AN80"/>
+      <c r="AO80"/>
+      <c r="AP80"/>
+      <c r="AQ80"/>
+      <c r="AR80"/>
+      <c r="AS80"/>
+      <c r="AT80"/>
+      <c r="AU80"/>
+      <c r="AV80"/>
+      <c r="AW80"/>
+      <c r="AX80"/>
+      <c r="AY80"/>
+      <c r="AZ80"/>
+      <c r="BA80"/>
+      <c r="BB80"/>
+      <c r="BC80"/>
+      <c r="BD80"/>
+      <c r="BE80"/>
+      <c r="BF80"/>
+      <c r="BG80"/>
+      <c r="BH80"/>
+      <c r="BI80"/>
+      <c r="BJ80"/>
+      <c r="BK80"/>
+      <c r="BL80"/>
+      <c r="BM80"/>
+      <c r="BN80"/>
+      <c r="BO80"/>
+      <c r="BP80"/>
+      <c r="BQ80"/>
+      <c r="BR80"/>
+      <c r="BS80"/>
+      <c r="BT80"/>
+      <c r="BU80"/>
+      <c r="BV80"/>
+      <c r="BW80"/>
+      <c r="BX80"/>
+      <c r="BY80"/>
+      <c r="BZ80"/>
+      <c r="CA80"/>
+      <c r="CB80"/>
+      <c r="CC80"/>
+      <c r="CD80"/>
+      <c r="CE80"/>
+      <c r="CF80"/>
+      <c r="CG80"/>
+      <c r="CH80"/>
+      <c r="CI80"/>
+      <c r="CJ80"/>
+      <c r="CK80"/>
+      <c r="CL80"/>
+      <c r="CM80"/>
+      <c r="CN80"/>
+      <c r="CO80"/>
+      <c r="CP80"/>
+      <c r="CQ80"/>
+      <c r="CR80"/>
+      <c r="CS80"/>
+      <c r="CT80"/>
+      <c r="CU80"/>
+      <c r="CV80"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
+      <c r="P81"/>
+      <c r="Q81"/>
+      <c r="R81"/>
+      <c r="S81"/>
+      <c r="T81"/>
+      <c r="U81"/>
+      <c r="V81"/>
+      <c r="W81"/>
+      <c r="X81"/>
+      <c r="Y81"/>
+      <c r="Z81"/>
+      <c r="AA81"/>
+      <c r="AB81"/>
+      <c r="AC81"/>
+      <c r="AD81"/>
+      <c r="AE81"/>
+      <c r="AF81"/>
+      <c r="AG81"/>
+      <c r="AH81"/>
+      <c r="AI81"/>
+      <c r="AJ81"/>
+      <c r="AK81"/>
+      <c r="AL81"/>
+      <c r="AM81"/>
+      <c r="AN81"/>
+      <c r="AO81"/>
+      <c r="AP81"/>
+      <c r="AQ81"/>
+      <c r="AR81"/>
+      <c r="AS81"/>
+      <c r="AT81"/>
+      <c r="AU81"/>
+      <c r="AV81"/>
+      <c r="AW81"/>
+      <c r="AX81"/>
+      <c r="AY81"/>
+      <c r="AZ81"/>
+      <c r="BA81"/>
+      <c r="BB81"/>
+      <c r="BC81"/>
+      <c r="BD81"/>
+      <c r="BE81"/>
+      <c r="BF81"/>
+      <c r="BG81"/>
+      <c r="BH81"/>
+      <c r="BI81"/>
+      <c r="BJ81"/>
+      <c r="BK81"/>
+      <c r="BL81"/>
+      <c r="BM81"/>
+      <c r="BN81"/>
+      <c r="BO81"/>
+      <c r="BP81"/>
+      <c r="BQ81"/>
+      <c r="BR81"/>
+      <c r="BS81"/>
+      <c r="BT81"/>
+      <c r="BU81"/>
+      <c r="BV81"/>
+      <c r="BW81"/>
+      <c r="BX81"/>
+      <c r="BY81"/>
+      <c r="BZ81"/>
+      <c r="CA81"/>
+      <c r="CB81"/>
+      <c r="CC81"/>
+      <c r="CD81"/>
+      <c r="CE81"/>
+      <c r="CF81"/>
+      <c r="CG81"/>
+      <c r="CH81"/>
+      <c r="CI81"/>
+      <c r="CJ81"/>
+      <c r="CK81"/>
+      <c r="CL81"/>
+      <c r="CM81"/>
+      <c r="CN81"/>
+      <c r="CO81"/>
+      <c r="CP81"/>
+      <c r="CQ81"/>
+      <c r="CR81"/>
+      <c r="CS81"/>
+      <c r="CT81"/>
+      <c r="CU81"/>
+      <c r="CV81"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+      <c r="P82"/>
+      <c r="Q82"/>
+      <c r="R82"/>
+      <c r="S82"/>
+      <c r="T82"/>
+      <c r="U82"/>
+      <c r="V82"/>
+      <c r="W82"/>
+      <c r="X82"/>
+      <c r="Y82"/>
+      <c r="Z82"/>
+      <c r="AA82"/>
+      <c r="AB82"/>
+      <c r="AC82"/>
+      <c r="AD82"/>
+      <c r="AE82"/>
+      <c r="AF82"/>
+      <c r="AG82"/>
+      <c r="AH82"/>
+      <c r="AI82"/>
+      <c r="AJ82"/>
+      <c r="AK82"/>
+      <c r="AL82"/>
+      <c r="AM82"/>
+      <c r="AN82"/>
+      <c r="AO82"/>
+      <c r="AP82"/>
+      <c r="AQ82"/>
+      <c r="AR82"/>
+      <c r="AS82"/>
+      <c r="AT82"/>
+      <c r="AU82"/>
+      <c r="AV82"/>
+      <c r="AW82"/>
+      <c r="AX82"/>
+      <c r="AY82"/>
+      <c r="AZ82"/>
+      <c r="BA82"/>
+      <c r="BB82"/>
+      <c r="BC82"/>
+      <c r="BD82"/>
+      <c r="BE82"/>
+      <c r="BF82"/>
+      <c r="BG82"/>
+      <c r="BH82"/>
+      <c r="BI82"/>
+      <c r="BJ82"/>
+      <c r="BK82"/>
+      <c r="BL82"/>
+      <c r="BM82"/>
+      <c r="BN82"/>
+      <c r="BO82"/>
+      <c r="BP82"/>
+      <c r="BQ82"/>
+      <c r="BR82"/>
+      <c r="BS82"/>
+      <c r="BT82"/>
+      <c r="BU82"/>
+      <c r="BV82"/>
+      <c r="BW82"/>
+      <c r="BX82"/>
+      <c r="BY82"/>
+      <c r="BZ82"/>
+      <c r="CA82"/>
+      <c r="CB82"/>
+      <c r="CC82"/>
+      <c r="CD82"/>
+      <c r="CE82"/>
+      <c r="CF82"/>
+      <c r="CG82"/>
+      <c r="CH82"/>
+      <c r="CI82"/>
+      <c r="CJ82"/>
+      <c r="CK82"/>
+      <c r="CL82"/>
+      <c r="CM82"/>
+      <c r="CN82"/>
+      <c r="CO82"/>
+      <c r="CP82"/>
+      <c r="CQ82"/>
+      <c r="CR82"/>
+      <c r="CS82"/>
+      <c r="CT82"/>
+      <c r="CU82"/>
+      <c r="CV82"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+      <c r="N83"/>
+      <c r="O83"/>
+      <c r="P83"/>
+      <c r="Q83"/>
+      <c r="R83"/>
+      <c r="S83"/>
+      <c r="T83"/>
+      <c r="U83"/>
+      <c r="V83"/>
+      <c r="W83"/>
+      <c r="X83"/>
+      <c r="Y83"/>
+      <c r="Z83"/>
+      <c r="AA83"/>
+      <c r="AB83"/>
+      <c r="AC83"/>
+      <c r="AD83"/>
+      <c r="AE83"/>
+      <c r="AF83"/>
+      <c r="AG83"/>
+      <c r="AH83"/>
+      <c r="AI83"/>
+      <c r="AJ83"/>
+      <c r="AK83"/>
+      <c r="AL83"/>
+      <c r="AM83"/>
+      <c r="AN83"/>
+      <c r="AO83"/>
+      <c r="AP83"/>
+      <c r="AQ83"/>
+      <c r="AR83"/>
+      <c r="AS83"/>
+      <c r="AT83"/>
+      <c r="AU83"/>
+      <c r="AV83"/>
+      <c r="AW83"/>
+      <c r="AX83"/>
+      <c r="AY83"/>
+      <c r="AZ83"/>
+      <c r="BA83"/>
+      <c r="BB83"/>
+      <c r="BC83"/>
+      <c r="BD83"/>
+      <c r="BE83"/>
+      <c r="BF83"/>
+      <c r="BG83"/>
+      <c r="BH83"/>
+      <c r="BI83"/>
+      <c r="BJ83"/>
+      <c r="BK83"/>
+      <c r="BL83"/>
+      <c r="BM83"/>
+      <c r="BN83"/>
+      <c r="BO83"/>
+      <c r="BP83"/>
+      <c r="BQ83"/>
+      <c r="BR83"/>
+      <c r="BS83"/>
+      <c r="BT83"/>
+      <c r="BU83"/>
+      <c r="BV83"/>
+      <c r="BW83"/>
+      <c r="BX83"/>
+      <c r="BY83"/>
+      <c r="BZ83"/>
+      <c r="CA83"/>
+      <c r="CB83"/>
+      <c r="CC83"/>
+      <c r="CD83"/>
+      <c r="CE83"/>
+      <c r="CF83"/>
+      <c r="CG83"/>
+      <c r="CH83"/>
+      <c r="CI83"/>
+      <c r="CJ83"/>
+      <c r="CK83"/>
+      <c r="CL83"/>
+      <c r="CM83"/>
+      <c r="CN83"/>
+      <c r="CO83"/>
+      <c r="CP83"/>
+      <c r="CQ83"/>
+      <c r="CR83"/>
+      <c r="CS83"/>
+      <c r="CT83"/>
+      <c r="CU83"/>
+      <c r="CV83"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>